<commit_message>
fix typo in MoA, preprocess dataset
</commit_message>
<xml_diff>
--- a/data/interim/BBBC021_v1_compound_smiles_moa.xlsx
+++ b/data/interim/BBBC021_v1_compound_smiles_moa.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c331f6d501fa4974/MADS/SIADS-699/BBBC021/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meine Ablage\SIADS-699\BBBC021 dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="58" documentId="8_{78BE70CC-254B-4986-843D-E99FDEB8C5E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B9C8B69F-4BEE-454F-89A3-1450152221AA}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E397D880-A1B5-4E16-A54D-8E728A24CA32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="435" windowWidth="24030" windowHeight="14535" xr2:uid="{3F49BC8C-4D44-4B4E-8566-7C4571767A8D}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="151">
   <si>
     <t>compound</t>
   </si>
@@ -371,9 +371,6 @@
   </si>
   <si>
     <t>CON</t>
-  </si>
-  <si>
-    <t>DNA demage</t>
   </si>
   <si>
     <t>ICI-182,780</t>
@@ -1924,37 +1921,37 @@
         <v>116</v>
       </c>
       <c r="C54" t="s">
-        <v>117</v>
+        <v>21</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>117</v>
+      </c>
+      <c r="B55" t="s">
         <v>118</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" t="s">
         <v>119</v>
-      </c>
-      <c r="C55" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>121</v>
+      </c>
+      <c r="B56" t="s">
         <v>122</v>
       </c>
-      <c r="B56" t="s">
-        <v>123</v>
-      </c>
       <c r="C56" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>123</v>
+      </c>
+      <c r="B57" t="s">
         <v>124</v>
-      </c>
-      <c r="B57" t="s">
-        <v>125</v>
       </c>
       <c r="C57" t="s">
         <v>75</v>
@@ -1962,21 +1959,21 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>125</v>
+      </c>
+      <c r="B58" t="s">
         <v>126</v>
       </c>
-      <c r="B58" t="s">
+      <c r="C58" t="s">
         <v>127</v>
-      </c>
-      <c r="C58" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>128</v>
+      </c>
+      <c r="B59" t="s">
         <v>129</v>
-      </c>
-      <c r="B59" t="s">
-        <v>130</v>
       </c>
       <c r="C59" t="s">
         <v>75</v>
@@ -1984,10 +1981,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>130</v>
+      </c>
+      <c r="B60" t="s">
         <v>131</v>
-      </c>
-      <c r="B60" t="s">
-        <v>132</v>
       </c>
       <c r="C60" t="s">
         <v>75</v>
@@ -1995,43 +1992,43 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>132</v>
+      </c>
+      <c r="B61" t="s">
         <v>133</v>
       </c>
-      <c r="B61" t="s">
-        <v>134</v>
-      </c>
       <c r="C61" t="s">
-        <v>117</v>
+        <v>21</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>134</v>
+      </c>
+      <c r="B62" t="s">
         <v>135</v>
       </c>
-      <c r="B62" t="s">
-        <v>136</v>
-      </c>
       <c r="C62" t="s">
-        <v>117</v>
+        <v>21</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>136</v>
+      </c>
+      <c r="B63" t="s">
         <v>137</v>
       </c>
-      <c r="B63" t="s">
-        <v>138</v>
-      </c>
       <c r="C63" t="s">
-        <v>117</v>
+        <v>21</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>138</v>
+      </c>
+      <c r="B64" t="s">
         <v>139</v>
-      </c>
-      <c r="B64" t="s">
-        <v>140</v>
       </c>
       <c r="C64" t="s">
         <v>9</v>
@@ -2039,10 +2036,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>140</v>
+      </c>
+      <c r="B65" t="s">
         <v>141</v>
-      </c>
-      <c r="B65" t="s">
-        <v>142</v>
       </c>
       <c r="C65" t="s">
         <v>9</v>
@@ -2050,10 +2047,10 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>142</v>
+      </c>
+      <c r="B66" t="s">
         <v>143</v>
-      </c>
-      <c r="B66" t="s">
-        <v>144</v>
       </c>
       <c r="C66" t="s">
         <v>75</v>
@@ -2061,21 +2058,21 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>144</v>
+      </c>
+      <c r="B67" t="s">
         <v>145</v>
       </c>
-      <c r="B67" t="s">
+      <c r="C67" t="s">
         <v>146</v>
-      </c>
-      <c r="C67" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>147</v>
+      </c>
+      <c r="B68" t="s">
         <v>148</v>
-      </c>
-      <c r="B68" t="s">
-        <v>149</v>
       </c>
       <c r="C68" t="s">
         <v>75</v>
@@ -2083,10 +2080,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>149</v>
+      </c>
+      <c r="B69" t="s">
         <v>150</v>
-      </c>
-      <c r="B69" t="s">
-        <v>151</v>
       </c>
       <c r="C69" t="s">
         <v>18</v>

</xml_diff>